<commit_message>
bot handles game day and bca mentions
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -1,66 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53cb9c05b082722/Documents/apa-rankings/data/slmatchups/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6A69D6BF8740D7030AA2DFD3533088B35299F730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{573B1835-B7A4-4AAF-BD97-FA102046F686}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="21105" yWindow="405" windowWidth="15150" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t>X1.2</t>
-  </si>
-  <si>
-    <t>X0.33</t>
-  </si>
-  <si>
-    <t>X1.0</t>
-  </si>
-  <si>
-    <t>X2.67</t>
-  </si>
-  <si>
-    <t>X1.8</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,46 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -402,178 +420,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="1" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="n">
         <v>1.5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>X0.33</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>X1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>X2.67</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>X1.8</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="F7" t="n">
         <v>1.46</v>
       </c>
-      <c r="D2" s="2">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.38</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.39</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.41</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.63</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.45</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.36</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.22</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.57</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.23</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.37</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.23</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.61</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.22</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.29</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.09</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.43</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1.2</v>
+      <c r="G7" t="n">
+        <v>1.19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated week 8 stats sum 22
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.43</v>
+        <v>1.42</v>
       </c>
       <c r="D2" t="n">
         <v>1.29</v>
       </c>
       <c r="E2" t="n">
-        <v>1.29</v>
+        <v>1.38</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -488,19 +488,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="E3" t="n">
         <v>1.36</v>
       </c>
       <c r="F3" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -516,16 +516,16 @@
         <v>1.42</v>
       </c>
       <c r="C4" t="n">
-        <v>1.53</v>
+        <v>1.54</v>
       </c>
       <c r="D4" t="n">
         <v>1.37</v>
       </c>
       <c r="E4" t="n">
-        <v>1.17</v>
+        <v>1.15</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>1.03</v>
       </c>
       <c r="G4" t="n">
         <v>0.5</v>
@@ -536,22 +536,22 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.57</v>
+        <v>1.38</v>
       </c>
       <c r="C5" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="D5" t="n">
-        <v>1.38</v>
+        <v>1.39</v>
       </c>
       <c r="E5" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F5" t="n">
-        <v>1.11</v>
+        <v>1.08</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="6">
@@ -562,13 +562,13 @@
         <v>1.57</v>
       </c>
       <c r="C6" t="n">
-        <v>1.77</v>
+        <v>1.64</v>
       </c>
       <c r="D6" t="n">
-        <v>1.68</v>
+        <v>1.62</v>
       </c>
       <c r="E6" t="n">
-        <v>1.26</v>
+        <v>1.28</v>
       </c>
       <c r="F6" t="n">
         <v>1.1</v>
@@ -595,10 +595,10 @@
         <v>2.38</v>
       </c>
       <c r="E7" t="n">
-        <v>2.04</v>
+        <v>2.08</v>
       </c>
       <c r="F7" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
sl now shows heatmap
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -597,6 +597,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added medians and modes
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="D2" t="n">
         <v>1.29</v>
@@ -486,19 +486,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.38</v>
+        <v>1.41</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="n">
-        <v>1.35</v>
+        <v>1.37</v>
       </c>
       <c r="F3" t="n">
-        <v>1.06</v>
+        <v>1.11</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -512,13 +512,13 @@
         <v>1.43</v>
       </c>
       <c r="C4" t="n">
-        <v>1.51</v>
+        <v>1.5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="E4" t="n">
-        <v>1.18</v>
+        <v>1.2</v>
       </c>
       <c r="F4" t="n">
         <v>1.03</v>
@@ -535,19 +535,19 @@
         <v>1.3</v>
       </c>
       <c r="C5" t="n">
-        <v>1.31</v>
+        <v>1.29</v>
       </c>
       <c r="D5" t="n">
-        <v>1.37</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="G5" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="6">
@@ -561,10 +561,10 @@
         <v>1.56</v>
       </c>
       <c r="D6" t="n">
-        <v>1.59</v>
+        <v>1.61</v>
       </c>
       <c r="E6" t="n">
-        <v>1.28</v>
+        <v>1.31</v>
       </c>
       <c r="F6" t="n">
         <v>1.14</v>
@@ -587,16 +587,16 @@
         <v>2.38</v>
       </c>
       <c r="E7" t="n">
-        <v>2.11</v>
+        <v>2.14</v>
       </c>
       <c r="F7" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fall 22 week 11 complete plus 9 ball skill level evals
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
       </c>
       <c r="E2" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="F2" t="n">
         <v>0.8</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,10 +495,10 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>1.31</v>
       </c>
       <c r="F3" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="G3" t="n">
         <v>0.83</v>
@@ -512,16 +512,16 @@
         <v>1.48</v>
       </c>
       <c r="C4" t="n">
-        <v>1.46</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="E4" t="n">
         <v>1.18</v>
       </c>
       <c r="F4" t="n">
-        <v>1.05</v>
+        <v>0.98</v>
       </c>
       <c r="G4" t="n">
         <v>0.55</v>
@@ -532,10 +532,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
       <c r="D5" t="n">
         <v>1.38</v>
@@ -547,7 +547,7 @@
         <v>1.07</v>
       </c>
       <c r="G5" t="n">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="6">
@@ -558,10 +558,10 @@
         <v>1.9</v>
       </c>
       <c r="C6" t="n">
-        <v>1.35</v>
+        <v>1.38</v>
       </c>
       <c r="D6" t="n">
-        <v>1.59</v>
+        <v>1.64</v>
       </c>
       <c r="E6" t="n">
         <v>1.29</v>
@@ -570,7 +570,7 @@
         <v>1.14</v>
       </c>
       <c r="G6" t="n">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="7">
@@ -590,13 +590,13 @@
         <v>2.09</v>
       </c>
       <c r="F7" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
         <v>1.18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fall 22 week 13 done
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,10 +466,10 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.28</v>
       </c>
       <c r="E2" t="n">
         <v>1.43</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.4</v>
+        <v>1.38</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,13 +495,13 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="F3" t="n">
         <v>1.28</v>
       </c>
       <c r="G3" t="n">
-        <v>0.83</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="4">
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.48</v>
+        <v>1.43</v>
       </c>
       <c r="C4" t="n">
         <v>1.44</v>
@@ -518,10 +518,10 @@
         <v>1.36</v>
       </c>
       <c r="E4" t="n">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="F4" t="n">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="G4" t="n">
         <v>0.55</v>
@@ -535,19 +535,19 @@
         <v>1.36</v>
       </c>
       <c r="C5" t="n">
-        <v>1.34</v>
+        <v>1.36</v>
       </c>
       <c r="D5" t="n">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="G5" t="n">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="6">
@@ -581,7 +581,7 @@
         <v>2.5</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>2.14</v>
       </c>
       <c r="D7" t="n">
         <v>2.27</v>
@@ -593,7 +593,7 @@
         <v>1.52</v>
       </c>
       <c r="G7" t="n">
-        <v>1.18</v>
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 14 complete
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="D2" t="n">
         <v>1.28</v>
@@ -492,16 +492,16 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="F3" t="n">
-        <v>1.28</v>
+        <v>1.31</v>
       </c>
       <c r="G3" t="n">
-        <v>0.71</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4">
@@ -512,16 +512,16 @@
         <v>1.43</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="E4" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="F4" t="n">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="G4" t="n">
         <v>0.55</v>
@@ -535,19 +535,19 @@
         <v>1.36</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="E5" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F5" t="n">
         <v>1.08</v>
       </c>
       <c r="G5" t="n">
-        <v>0.54</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="6">
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>1.4</v>
+        <v>1.35</v>
       </c>
       <c r="D6" t="n">
         <v>1.64</v>
@@ -570,7 +570,7 @@
         <v>1.14</v>
       </c>
       <c r="G6" t="n">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="7">
@@ -581,16 +581,16 @@
         <v>2.5</v>
       </c>
       <c r="C7" t="n">
-        <v>2.14</v>
+        <v>2.12</v>
       </c>
       <c r="D7" t="n">
         <v>2.27</v>
       </c>
       <c r="E7" t="n">
-        <v>2.09</v>
+        <v>2.06</v>
       </c>
       <c r="F7" t="n">
-        <v>1.52</v>
+        <v>1.54</v>
       </c>
       <c r="G7" t="n">
         <v>1.2</v>

</xml_diff>

<commit_message>
spring 23 week 7 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,16 +466,16 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="D2" t="n">
         <v>1.31</v>
       </c>
       <c r="E2" t="n">
-        <v>1.33</v>
+        <v>1.26</v>
       </c>
       <c r="F2" t="n">
-        <v>0.77</v>
+        <v>0.71</v>
       </c>
       <c r="G2" t="n">
         <v>0.5</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -512,13 +512,13 @@
         <v>1.43</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
         <v>1.35</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23</v>
+        <v>1.21</v>
       </c>
       <c r="F4" t="n">
         <v>1.02</v>
@@ -532,13 +532,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.39</v>
+        <v>1.47</v>
       </c>
       <c r="C5" t="n">
         <v>1.37</v>
       </c>
       <c r="D5" t="n">
-        <v>1.33</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -547,7 +547,7 @@
         <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="6">
@@ -555,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>2.07</v>
       </c>
       <c r="C6" t="n">
         <v>1.39</v>
@@ -564,13 +564,13 @@
         <v>1.59</v>
       </c>
       <c r="E6" t="n">
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
       <c r="F6" t="n">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
       <c r="G6" t="n">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>2.2</v>
       </c>
       <c r="E7" t="n">
-        <v>1.95</v>
+        <v>1.98</v>
       </c>
       <c r="F7" t="n">
-        <v>1.52</v>
+        <v>1.53</v>
       </c>
       <c r="G7" t="n">
         <v>1.2</v>

</xml_diff>

<commit_message>
spring week 8 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,10 +466,10 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="D2" t="n">
-        <v>1.31</v>
+        <v>1.28</v>
       </c>
       <c r="E2" t="n">
         <v>1.26</v>
@@ -492,16 +492,16 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="E3" t="n">
-        <v>1.27</v>
+        <v>1.28</v>
       </c>
       <c r="F3" t="n">
         <v>1.26</v>
       </c>
       <c r="G3" t="n">
-        <v>0.58</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="4">
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.43</v>
+        <v>1.46</v>
       </c>
       <c r="C4" t="n">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
         <v>1.35</v>
       </c>
       <c r="E4" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>0.6</v>
@@ -535,10 +535,10 @@
         <v>1.47</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -547,7 +547,7 @@
         <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.63</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="6">
@@ -561,7 +561,7 @@
         <v>1.39</v>
       </c>
       <c r="D6" t="n">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="E6" t="n">
         <v>1.29</v>
@@ -581,13 +581,13 @@
         <v>2.5</v>
       </c>
       <c r="C7" t="n">
-        <v>2.33</v>
+        <v>2.38</v>
       </c>
       <c r="D7" t="n">
         <v>2.2</v>
       </c>
       <c r="E7" t="n">
-        <v>1.98</v>
+        <v>1.93</v>
       </c>
       <c r="F7" t="n">
         <v>1.53</v>

</xml_diff>

<commit_message>
spring 23 week 10 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.42</v>
       </c>
       <c r="D2" t="n">
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
       <c r="E2" t="n">
         <v>1.26</v>
@@ -486,22 +486,22 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.41</v>
+        <v>1.42</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
         <v>1.28</v>
       </c>
       <c r="F3" t="n">
-        <v>1.22</v>
+        <v>1.24</v>
       </c>
       <c r="G3" t="n">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.46</v>
+        <v>1.43</v>
       </c>
       <c r="C4" t="n">
-        <v>1.45</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E4" t="n">
         <v>1.23</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>1.04</v>
       </c>
       <c r="G4" t="n">
         <v>0.6899999999999999</v>
@@ -544,10 +544,10 @@
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="6">
@@ -558,10 +558,10 @@
         <v>2.07</v>
       </c>
       <c r="C6" t="n">
-        <v>1.44</v>
+        <v>1.42</v>
       </c>
       <c r="D6" t="n">
-        <v>1.6</v>
+        <v>1.56</v>
       </c>
       <c r="E6" t="n">
         <v>1.29</v>
@@ -581,19 +581,19 @@
         <v>2.5</v>
       </c>
       <c r="C7" t="n">
-        <v>2.38</v>
+        <v>2.43</v>
       </c>
       <c r="D7" t="n">
         <v>2.06</v>
       </c>
       <c r="E7" t="n">
-        <v>1.89</v>
+        <v>1.91</v>
       </c>
       <c r="F7" t="n">
         <v>1.51</v>
       </c>
       <c r="G7" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
march 28 inputs but nine ball update failed
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.39</v>
       </c>
       <c r="D2" t="n">
-        <v>1.29</v>
+        <v>1.31</v>
       </c>
       <c r="E2" t="n">
         <v>1.3</v>
@@ -492,13 +492,13 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.42</v>
       </c>
       <c r="E3" t="n">
         <v>1.28</v>
       </c>
       <c r="F3" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="G3" t="n">
         <v>0.5</v>
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.43</v>
+        <v>1.4</v>
       </c>
       <c r="C4" t="n">
-        <v>1.43</v>
+        <v>1.42</v>
       </c>
       <c r="D4" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E4" t="n">
         <v>1.24</v>
       </c>
       <c r="F4" t="n">
-        <v>1.04</v>
+        <v>1.07</v>
       </c>
       <c r="G4" t="n">
         <v>0.76</v>
@@ -535,19 +535,19 @@
         <v>1.45</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
         <v>1.32</v>
       </c>
       <c r="E5" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F5" t="n">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="6">
@@ -558,19 +558,19 @@
         <v>2.07</v>
       </c>
       <c r="C6" t="n">
-        <v>1.42</v>
+        <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.56</v>
+        <v>1.53</v>
       </c>
       <c r="E6" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="F6" t="n">
         <v>1.14</v>
       </c>
       <c r="G6" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>1.94</v>
       </c>
       <c r="E7" t="n">
-        <v>1.94</v>
+        <v>1.96</v>
       </c>
       <c r="F7" t="n">
-        <v>1.51</v>
+        <v>1.5</v>
       </c>
       <c r="G7" t="n">
         <v>1.18</v>

</xml_diff>

<commit_message>
spring 23 week 13 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -472,10 +472,10 @@
         <v>1.31</v>
       </c>
       <c r="E2" t="n">
-        <v>1.3</v>
+        <v>1.32</v>
       </c>
       <c r="F2" t="n">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
       <c r="G2" t="n">
         <v>0.5</v>
@@ -492,10 +492,10 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="E3" t="n">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
       <c r="F3" t="n">
         <v>1.23</v>
@@ -512,7 +512,7 @@
         <v>1.4</v>
       </c>
       <c r="C4" t="n">
-        <v>1.42</v>
+        <v>1.4</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
@@ -521,7 +521,7 @@
         <v>1.24</v>
       </c>
       <c r="F4" t="n">
-        <v>1.07</v>
+        <v>1.09</v>
       </c>
       <c r="G4" t="n">
         <v>0.76</v>
@@ -535,16 +535,16 @@
         <v>1.45</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
         <v>1.32</v>
       </c>
       <c r="E5" t="n">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="G5" t="n">
         <v>0.65</v>
@@ -561,13 +561,13 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.53</v>
+        <v>1.52</v>
       </c>
       <c r="E6" t="n">
-        <v>1.3</v>
+        <v>1.31</v>
       </c>
       <c r="F6" t="n">
-        <v>1.14</v>
+        <v>1.15</v>
       </c>
       <c r="G6" t="n">
         <v>1.04</v>

</xml_diff>

<commit_message>
spring 23 week 14 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="D2" t="n">
         <v>1.31</v>
       </c>
       <c r="E2" t="n">
-        <v>1.32</v>
+        <v>1.3</v>
       </c>
       <c r="F2" t="n">
         <v>0.73</v>
@@ -486,13 +486,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="E3" t="n">
         <v>1.26</v>
@@ -518,7 +518,7 @@
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.24</v>
+        <v>1.25</v>
       </c>
       <c r="F4" t="n">
         <v>1.09</v>
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.45</v>
+        <v>1.48</v>
       </c>
       <c r="C5" t="n">
         <v>1.38</v>
@@ -547,7 +547,7 @@
         <v>1.05</v>
       </c>
       <c r="G5" t="n">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="6">
@@ -564,7 +564,7 @@
         <v>1.52</v>
       </c>
       <c r="E6" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.15</v>
@@ -587,7 +587,7 @@
         <v>1.94</v>
       </c>
       <c r="E7" t="n">
-        <v>1.96</v>
+        <v>1.94</v>
       </c>
       <c r="F7" t="n">
         <v>1.5</v>

</xml_diff>

<commit_message>
spring 23 week 15 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.38</v>
       </c>
       <c r="D2" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="E2" t="n">
         <v>1.3</v>
@@ -495,7 +495,7 @@
         <v>1.44</v>
       </c>
       <c r="E3" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="F3" t="n">
         <v>1.23</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.4</v>
+        <v>1.42</v>
       </c>
       <c r="C4" t="n">
         <v>1.4</v>
@@ -521,7 +521,7 @@
         <v>1.25</v>
       </c>
       <c r="F4" t="n">
-        <v>1.09</v>
+        <v>1.08</v>
       </c>
       <c r="G4" t="n">
         <v>0.76</v>
@@ -535,10 +535,10 @@
         <v>1.48</v>
       </c>
       <c r="C5" t="n">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -547,7 +547,7 @@
         <v>1.05</v>
       </c>
       <c r="G5" t="n">
-        <v>0.68</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="6">
@@ -561,7 +561,7 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.52</v>
+        <v>1.53</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>
@@ -587,10 +587,10 @@
         <v>1.94</v>
       </c>
       <c r="E7" t="n">
-        <v>1.94</v>
+        <v>1.92</v>
       </c>
       <c r="F7" t="n">
-        <v>1.5</v>
+        <v>1.51</v>
       </c>
       <c r="G7" t="n">
         <v>1.18</v>

</xml_diff>

<commit_message>
spring 23 inputs complete
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -478,7 +478,7 @@
         <v>0.73</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>1.44</v>
       </c>
       <c r="E3" t="n">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="F3" t="n">
         <v>1.23</v>
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="C4" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="G4" t="n">
         <v>0.76</v>
@@ -535,19 +535,19 @@
         <v>1.48</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
       <c r="G5" t="n">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6">
@@ -561,7 +561,7 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.53</v>
+        <v>1.55</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>
@@ -570,7 +570,7 @@
         <v>1.15</v>
       </c>
       <c r="G6" t="n">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="7">
@@ -578,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="C7" t="n">
         <v>2.43</v>
@@ -590,7 +590,7 @@
         <v>1.92</v>
       </c>
       <c r="F7" t="n">
-        <v>1.51</v>
+        <v>1.49</v>
       </c>
       <c r="G7" t="n">
         <v>1.18</v>

</xml_diff>

<commit_message>
summer 23 week 1 input
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,10 +469,10 @@
         <v>1.38</v>
       </c>
       <c r="D2" t="n">
-        <v>1.3</v>
+        <v>1.27</v>
       </c>
       <c r="E2" t="n">
-        <v>1.3</v>
+        <v>1.33</v>
       </c>
       <c r="F2" t="n">
         <v>0.73</v>
@@ -509,10 +509,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
       <c r="C4" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
@@ -521,7 +521,7 @@
         <v>1.24</v>
       </c>
       <c r="F4" t="n">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="G4" t="n">
         <v>0.76</v>
@@ -532,19 +532,19 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.48</v>
+        <v>1.42</v>
       </c>
       <c r="C5" t="n">
         <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
       <c r="G5" t="n">
         <v>0.7</v>
@@ -561,7 +561,7 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.55</v>
+        <v>1.52</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>

</xml_diff>

<commit_message>
summer 23 week 2 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="E3" t="n">
         <v>1.26</v>
@@ -538,13 +538,13 @@
         <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="G5" t="n">
         <v>0.7</v>
@@ -564,7 +564,7 @@
         <v>1.52</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
summer 23 week 5 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,10 +492,10 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
       <c r="E3" t="n">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
       <c r="F3" t="n">
         <v>1.23</v>
@@ -512,7 +512,7 @@
         <v>1.46</v>
       </c>
       <c r="C4" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
@@ -535,7 +535,7 @@
         <v>1.42</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
         <v>1.31</v>
@@ -561,7 +561,7 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.52</v>
+        <v>1.53</v>
       </c>
       <c r="E6" t="n">
         <v>1.33</v>
@@ -570,7 +570,7 @@
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.04</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
sum 23 week 6 input and game day reaction refactor
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>1.38</v>
       </c>
       <c r="D2" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="E2" t="n">
         <v>1.33</v>
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="E3" t="n">
         <v>1.26</v>
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.46</v>
+        <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.41</v>
+        <v>1.42</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="G4" t="n">
         <v>0.89</v>
@@ -561,7 +561,7 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.53</v>
+        <v>1.55</v>
       </c>
       <c r="E6" t="n">
         <v>1.33</v>
@@ -570,7 +570,7 @@
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.92</v>
       </c>
       <c r="F7" t="n">
-        <v>1.51</v>
+        <v>1.54</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
sum 23 week 7 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -495,10 +495,10 @@
         <v>1.43</v>
       </c>
       <c r="E3" t="n">
-        <v>1.26</v>
+        <v>1.28</v>
       </c>
       <c r="F3" t="n">
-        <v>1.23</v>
+        <v>1.19</v>
       </c>
       <c r="G3" t="n">
         <v>0.5</v>
@@ -518,7 +518,7 @@
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
       <c r="F4" t="n">
         <v>1.06</v>
@@ -535,7 +535,7 @@
         <v>1.42</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="D5" t="n">
         <v>1.31</v>
@@ -558,7 +558,7 @@
         <v>2.07</v>
       </c>
       <c r="C6" t="n">
-        <v>1.46</v>
+        <v>1.5</v>
       </c>
       <c r="D6" t="n">
         <v>1.55</v>
@@ -570,7 +570,7 @@
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -587,7 +587,7 @@
         <v>1.83</v>
       </c>
       <c r="E7" t="n">
-        <v>1.92</v>
+        <v>1.93</v>
       </c>
       <c r="F7" t="n">
         <v>1.54</v>

</xml_diff>

<commit_message>
caught up through july 4th
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.38</v>
+        <v>1.39</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
       </c>
       <c r="E2" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
       <c r="F2" t="n">
         <v>0.73</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.46</v>
+        <v>1.43</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -501,7 +501,7 @@
         <v>1.19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4">
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.42</v>
+        <v>1.36</v>
       </c>
       <c r="C5" t="n">
         <v>1.36</v>
@@ -561,16 +561,16 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.55</v>
+        <v>1.57</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="F6" t="n">
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="7">
@@ -581,7 +581,7 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.43</v>
+        <v>2.27</v>
       </c>
       <c r="D7" t="n">
         <v>1.83</v>
@@ -590,7 +590,7 @@
         <v>1.93</v>
       </c>
       <c r="F7" t="n">
-        <v>1.54</v>
+        <v>1.52</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
summer 23 week 9 input
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,10 +492,10 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.43</v>
+        <v>1.42</v>
       </c>
       <c r="E3" t="n">
-        <v>1.28</v>
+        <v>1.27</v>
       </c>
       <c r="F3" t="n">
         <v>1.19</v>
@@ -512,16 +512,16 @@
         <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.42</v>
+        <v>1.44</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="F4" t="n">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
       <c r="G4" t="n">
         <v>0.89</v>
@@ -535,7 +535,7 @@
         <v>1.36</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
         <v>1.31</v>
@@ -561,16 +561,16 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.57</v>
+        <v>1.56</v>
       </c>
       <c r="E6" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.93</v>
       </c>
       <c r="F7" t="n">
-        <v>1.52</v>
+        <v>1.51</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
summer 23 week 11 updated
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -472,7 +472,7 @@
         <v>1.25</v>
       </c>
       <c r="E2" t="n">
-        <v>1.36</v>
+        <v>1.29</v>
       </c>
       <c r="F2" t="n">
         <v>0.73</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -512,19 +512,19 @@
         <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.42</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="F4" t="n">
         <v>1.07</v>
       </c>
       <c r="G4" t="n">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="5">
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.36</v>
+        <v>1.43</v>
       </c>
       <c r="C5" t="n">
         <v>1.37</v>
@@ -547,7 +547,7 @@
         <v>1.04</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="6">
@@ -570,7 +570,7 @@
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.02</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="7">
@@ -584,13 +584,13 @@
         <v>2.27</v>
       </c>
       <c r="D7" t="n">
-        <v>1.83</v>
+        <v>1.89</v>
       </c>
       <c r="E7" t="n">
         <v>1.93</v>
       </c>
       <c r="F7" t="n">
-        <v>1.51</v>
+        <v>1.48</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
summer 23 week 13 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.39</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="E2" t="n">
         <v>1.29</v>
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="E3" t="n">
         <v>1.27</v>
@@ -509,10 +509,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.49</v>
+        <v>1.48</v>
       </c>
       <c r="C4" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
@@ -524,7 +524,7 @@
         <v>1.07</v>
       </c>
       <c r="G4" t="n">
-        <v>0.84</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5">
@@ -535,7 +535,7 @@
         <v>1.43</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
         <v>1.31</v>
@@ -544,10 +544,10 @@
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="G5" t="n">
-        <v>0.71</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="6">
@@ -561,16 +561,16 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="F6" t="n">
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="7">
@@ -584,13 +584,13 @@
         <v>2.27</v>
       </c>
       <c r="D7" t="n">
-        <v>1.89</v>
+        <v>1.8</v>
       </c>
       <c r="E7" t="n">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
summer 23 week 14 complete
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="D2" t="n">
         <v>1.26</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.44</v>
+        <v>1.46</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -501,7 +501,7 @@
         <v>1.19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="4">
@@ -512,7 +512,7 @@
         <v>1.48</v>
       </c>
       <c r="C4" t="n">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
@@ -521,7 +521,7 @@
         <v>1.27</v>
       </c>
       <c r="F4" t="n">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="G4" t="n">
         <v>0.9</v>
@@ -538,13 +538,13 @@
         <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="G5" t="n">
         <v>0.68</v>
@@ -561,16 +561,16 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.57</v>
+        <v>1.56</v>
       </c>
       <c r="E6" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="F6" t="n">
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="7">
@@ -581,7 +581,7 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.27</v>
+        <v>2.35</v>
       </c>
       <c r="D7" t="n">
         <v>1.8</v>
@@ -590,7 +590,7 @@
         <v>1.96</v>
       </c>
       <c r="F7" t="n">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 23 week 1 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
         <v>1.27</v>
@@ -512,13 +512,13 @@
         <v>1.48</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
         <v>1.34</v>
       </c>
       <c r="E4" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="F4" t="n">
         <v>1.08</v>
@@ -538,16 +538,16 @@
         <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.3</v>
+        <v>1.32</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="G5" t="n">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="6">
@@ -564,13 +564,13 @@
         <v>1.56</v>
       </c>
       <c r="E6" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="F6" t="n">
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="7">
@@ -587,7 +587,7 @@
         <v>1.8</v>
       </c>
       <c r="E7" t="n">
-        <v>1.96</v>
+        <v>1.97</v>
       </c>
       <c r="F7" t="n">
         <v>1.46</v>

</xml_diff>

<commit_message>
fall 23 week 2 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="D2" t="n">
         <v>1.26</v>
@@ -495,13 +495,13 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.27</v>
+        <v>1.29</v>
       </c>
       <c r="F3" t="n">
         <v>1.19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.53</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         <v>1.25</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08</v>
+        <v>1.1</v>
       </c>
       <c r="G4" t="n">
         <v>0.9</v>
@@ -535,7 +535,7 @@
         <v>1.43</v>
       </c>
       <c r="C5" t="n">
-        <v>1.38</v>
+        <v>1.35</v>
       </c>
       <c r="D5" t="n">
         <v>1.32</v>
@@ -561,7 +561,7 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.56</v>
+        <v>1.55</v>
       </c>
       <c r="E6" t="n">
         <v>1.34</v>
@@ -570,7 +570,7 @@
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="7">
@@ -581,7 +581,7 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.35</v>
+        <v>2.22</v>
       </c>
       <c r="D7" t="n">
         <v>1.8</v>
@@ -590,7 +590,7 @@
         <v>1.97</v>
       </c>
       <c r="F7" t="n">
-        <v>1.46</v>
+        <v>1.44</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 13 week 3 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.37</v>
       </c>
       <c r="D2" t="n">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
       <c r="E2" t="n">
         <v>1.29</v>
@@ -509,22 +509,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="C4" t="n">
         <v>1.45</v>
       </c>
       <c r="D4" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="E4" t="n">
         <v>1.25</v>
       </c>
       <c r="F4" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="5">
@@ -538,16 +538,16 @@
         <v>1.35</v>
       </c>
       <c r="D5" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="G5" t="n">
-        <v>0.67</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="6">
@@ -584,13 +584,13 @@
         <v>2.22</v>
       </c>
       <c r="D7" t="n">
-        <v>1.8</v>
+        <v>1.86</v>
       </c>
       <c r="E7" t="n">
-        <v>1.97</v>
+        <v>1.9</v>
       </c>
       <c r="F7" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 23 week 4 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
       </c>
       <c r="E2" t="n">
-        <v>1.29</v>
+        <v>1.24</v>
       </c>
       <c r="F2" t="n">
         <v>0.73</v>
@@ -486,16 +486,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="E3" t="n">
-        <v>1.29</v>
+        <v>1.27</v>
       </c>
       <c r="F3" t="n">
         <v>1.19</v>
@@ -512,16 +512,16 @@
         <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="D4" t="n">
         <v>1.33</v>
       </c>
       <c r="E4" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08</v>
+        <v>1.09</v>
       </c>
       <c r="G4" t="n">
         <v>0.86</v>
@@ -532,22 +532,22 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.43</v>
+        <v>1.48</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="G5" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="6">
@@ -561,16 +561,16 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.55</v>
+        <v>1.53</v>
       </c>
       <c r="E6" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>1.86</v>
       </c>
       <c r="E7" t="n">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="F7" t="n">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 23 week 5 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.47</v>
+        <v>1.46</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -521,10 +521,10 @@
         <v>1.24</v>
       </c>
       <c r="F4" t="n">
-        <v>1.09</v>
+        <v>1.08</v>
       </c>
       <c r="G4" t="n">
-        <v>0.86</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="5">
@@ -561,7 +561,7 @@
         <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.53</v>
+        <v>1.54</v>
       </c>
       <c r="E6" t="n">
         <v>1.33</v>
@@ -570,7 +570,7 @@
         <v>1.16</v>
       </c>
       <c r="G6" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="7">
@@ -584,13 +584,13 @@
         <v>2.22</v>
       </c>
       <c r="D7" t="n">
-        <v>1.86</v>
+        <v>1.77</v>
       </c>
       <c r="E7" t="n">
         <v>1.92</v>
       </c>
       <c r="F7" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 23 week 6 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -498,7 +498,7 @@
         <v>1.27</v>
       </c>
       <c r="F3" t="n">
-        <v>1.19</v>
+        <v>1.21</v>
       </c>
       <c r="G3" t="n">
         <v>0.61</v>
@@ -518,7 +518,7 @@
         <v>1.33</v>
       </c>
       <c r="E4" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="F4" t="n">
         <v>1.08</v>
@@ -535,10 +535,10 @@
         <v>1.48</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -547,7 +547,7 @@
         <v>1.03</v>
       </c>
       <c r="G5" t="n">
-        <v>0.72</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6">
@@ -558,7 +558,7 @@
         <v>2.07</v>
       </c>
       <c r="C6" t="n">
-        <v>1.5</v>
+        <v>1.47</v>
       </c>
       <c r="D6" t="n">
         <v>1.54</v>
@@ -584,10 +584,10 @@
         <v>2.22</v>
       </c>
       <c r="D7" t="n">
-        <v>1.77</v>
+        <v>1.78</v>
       </c>
       <c r="E7" t="n">
-        <v>1.92</v>
+        <v>1.89</v>
       </c>
       <c r="F7" t="n">
         <v>1.45</v>

</xml_diff>

<commit_message>
fall 23 week 7 updates
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -501,7 +501,7 @@
         <v>1.21</v>
       </c>
       <c r="G3" t="n">
-        <v>0.61</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="4">
@@ -561,16 +561,16 @@
         <v>1.47</v>
       </c>
       <c r="D6" t="n">
-        <v>1.54</v>
+        <v>1.55</v>
       </c>
       <c r="E6" t="n">
         <v>1.33</v>
       </c>
       <c r="F6" t="n">
-        <v>1.16</v>
+        <v>1.17</v>
       </c>
       <c r="G6" t="n">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="7">
@@ -581,7 +581,7 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.22</v>
+        <v>2.11</v>
       </c>
       <c r="D7" t="n">
         <v>1.78</v>
@@ -590,7 +590,7 @@
         <v>1.89</v>
       </c>
       <c r="F7" t="n">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="G7" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 23 week 10 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -498,7 +498,7 @@
         <v>1.27</v>
       </c>
       <c r="F3" t="n">
-        <v>1.21</v>
+        <v>1.23</v>
       </c>
       <c r="G3" t="n">
         <v>0.68</v>
@@ -518,7 +518,7 @@
         <v>1.33</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
         <v>1.08</v>
@@ -538,13 +538,13 @@
         <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="G5" t="n">
         <v>0.76</v>
@@ -558,16 +558,16 @@
         <v>2.07</v>
       </c>
       <c r="C6" t="n">
-        <v>1.47</v>
+        <v>1.46</v>
       </c>
       <c r="D6" t="n">
         <v>1.55</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.31</v>
       </c>
       <c r="F6" t="n">
-        <v>1.17</v>
+        <v>1.18</v>
       </c>
       <c r="G6" t="n">
         <v>1.04</v>

</xml_diff>

<commit_message>
fall 23 week 12 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.35</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
       <c r="E2" t="n">
         <v>1.24</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.47</v>
+        <v>1.48</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,10 +495,10 @@
         <v>1.39</v>
       </c>
       <c r="E3" t="n">
-        <v>1.27</v>
+        <v>1.29</v>
       </c>
       <c r="F3" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="G3" t="n">
         <v>0.68</v>
@@ -509,16 +509,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.49</v>
+        <v>1.47</v>
       </c>
       <c r="C4" t="n">
-        <v>1.46</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="F4" t="n">
         <v>1.08</v>
@@ -535,19 +535,19 @@
         <v>1.48</v>
       </c>
       <c r="C5" t="n">
-        <v>1.38</v>
+        <v>1.35</v>
       </c>
       <c r="D5" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
       <c r="G5" t="n">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="6">
@@ -561,10 +561,10 @@
         <v>1.46</v>
       </c>
       <c r="D6" t="n">
-        <v>1.55</v>
+        <v>1.54</v>
       </c>
       <c r="E6" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.18</v>
@@ -587,13 +587,13 @@
         <v>1.78</v>
       </c>
       <c r="E7" t="n">
-        <v>1.89</v>
+        <v>1.87</v>
       </c>
       <c r="F7" t="n">
         <v>1.46</v>
       </c>
       <c r="G7" t="n">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 23 week 14 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,16 +466,16 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="D2" t="n">
         <v>1.27</v>
       </c>
       <c r="E2" t="n">
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
       <c r="F2" t="n">
-        <v>0.73</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G2" t="n">
         <v>0.4</v>
@@ -486,19 +486,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="F3" t="n">
-        <v>1.22</v>
+        <v>1.19</v>
       </c>
       <c r="G3" t="n">
         <v>0.68</v>
@@ -521,7 +521,7 @@
         <v>1.23</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="G4" t="n">
         <v>0.91</v>
@@ -532,22 +532,22 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.48</v>
+        <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.04</v>
+        <v>1.02</v>
       </c>
       <c r="G5" t="n">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6">
@@ -555,16 +555,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>2.07</v>
+        <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.46</v>
+        <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.54</v>
+        <v>1.56</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.18</v>

</xml_diff>

<commit_message>
fall 23 week 15 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.34</v>
       </c>
       <c r="D2" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="E2" t="n">
         <v>1.2</v>
@@ -492,13 +492,13 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="E3" t="n">
         <v>1.28</v>
       </c>
       <c r="F3" t="n">
-        <v>1.19</v>
+        <v>1.21</v>
       </c>
       <c r="G3" t="n">
         <v>0.68</v>
@@ -509,10 +509,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.47</v>
+        <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.45</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
@@ -521,10 +521,10 @@
         <v>1.23</v>
       </c>
       <c r="F4" t="n">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
       <c r="G4" t="n">
-        <v>0.91</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -535,16 +535,16 @@
         <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="G5" t="n">
         <v>0.76</v>
@@ -558,10 +558,10 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.5</v>
+        <v>1.47</v>
       </c>
       <c r="D6" t="n">
-        <v>1.56</v>
+        <v>1.54</v>
       </c>
       <c r="E6" t="n">
         <v>1.33</v>
@@ -570,7 +570,7 @@
         <v>1.18</v>
       </c>
       <c r="G6" t="n">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="7">
@@ -584,13 +584,13 @@
         <v>2.11</v>
       </c>
       <c r="D7" t="n">
-        <v>1.78</v>
+        <v>1.71</v>
       </c>
       <c r="E7" t="n">
         <v>1.87</v>
       </c>
       <c r="F7" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
         <v>1.18</v>

</xml_diff>

<commit_message>
week 2 spring 24
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
@@ -495,7 +495,7 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="F3" t="n">
         <v>1.21</v>
@@ -518,7 +518,7 @@
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
@@ -535,19 +535,19 @@
         <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="G5" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="6">
@@ -561,7 +561,7 @@
         <v>1.47</v>
       </c>
       <c r="D6" t="n">
-        <v>1.52</v>
+        <v>1.51</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>
@@ -570,7 +570,7 @@
         <v>1.18</v>
       </c>
       <c r="G6" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>1.71</v>
       </c>
       <c r="E7" t="n">
-        <v>1.84</v>
+        <v>1.86</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="G7" t="n">
         <v>1.18</v>

</xml_diff>

<commit_message>
spring 24 week 3 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.34</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="E2" t="n">
         <v>1.2</v>
@@ -495,13 +495,13 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>1.31</v>
       </c>
       <c r="F3" t="n">
         <v>1.21</v>
       </c>
       <c r="G3" t="n">
-        <v>0.68</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="4">
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.49</v>
+        <v>1.52</v>
       </c>
       <c r="C4" t="n">
         <v>1.44</v>
@@ -518,13 +518,13 @@
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="5">
@@ -535,16 +535,16 @@
         <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="G5" t="n">
         <v>0.77</v>
@@ -564,10 +564,10 @@
         <v>1.51</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="G6" t="n">
         <v>1.01</v>
@@ -581,10 +581,10 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.11</v>
+        <v>2.15</v>
       </c>
       <c r="D7" t="n">
-        <v>1.71</v>
+        <v>1.76</v>
       </c>
       <c r="E7" t="n">
         <v>1.86</v>

</xml_diff>

<commit_message>
spring 24 week 5 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.34</v>
       </c>
       <c r="D2" t="n">
-        <v>1.23</v>
+        <v>1.24</v>
       </c>
       <c r="E2" t="n">
         <v>1.2</v>
@@ -495,10 +495,10 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="F3" t="n">
-        <v>1.21</v>
+        <v>1.23</v>
       </c>
       <c r="G3" t="n">
         <v>0.65</v>
@@ -509,10 +509,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
@@ -521,7 +521,7 @@
         <v>1.23</v>
       </c>
       <c r="F4" t="n">
-        <v>1.1</v>
+        <v>1.11</v>
       </c>
       <c r="G4" t="n">
         <v>0.96</v>
@@ -535,7 +535,7 @@
         <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -544,7 +544,7 @@
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="G5" t="n">
         <v>0.77</v>
@@ -558,13 +558,13 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="D6" t="n">
-        <v>1.51</v>
+        <v>1.49</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>
@@ -584,7 +584,7 @@
         <v>2.15</v>
       </c>
       <c r="D7" t="n">
-        <v>1.76</v>
+        <v>1.77</v>
       </c>
       <c r="E7" t="n">
         <v>1.86</v>

</xml_diff>

<commit_message>
spting 24 week 6 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.34</v>
       </c>
       <c r="D2" t="n">
-        <v>1.24</v>
+        <v>1.25</v>
       </c>
       <c r="E2" t="n">
         <v>1.2</v>
@@ -495,7 +495,7 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F3" t="n">
         <v>1.23</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.49</v>
+        <v>1.47</v>
       </c>
       <c r="C4" t="n">
         <v>1.45</v>
@@ -535,7 +535,7 @@
         <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -570,7 +570,7 @@
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="7">
@@ -590,10 +590,10 @@
         <v>1.86</v>
       </c>
       <c r="F7" t="n">
-        <v>1.49</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spr 24 week 10 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
       </c>
       <c r="E2" t="n">
-        <v>1.2</v>
+        <v>1.16</v>
       </c>
       <c r="F2" t="n">
         <v>0.6899999999999999</v>
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
         <v>1.33</v>
@@ -512,16 +512,16 @@
         <v>1.48</v>
       </c>
       <c r="C4" t="n">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="F4" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="G4" t="n">
         <v>0.97</v>
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.53</v>
+        <v>1.58</v>
       </c>
       <c r="C5" t="n">
         <v>1.32</v>
@@ -561,10 +561,10 @@
         <v>1.48</v>
       </c>
       <c r="D6" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="E6" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.2</v>
@@ -593,7 +593,7 @@
         <v>1.48</v>
       </c>
       <c r="G7" t="n">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spring 24 week 11 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -495,7 +495,7 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -512,7 +512,7 @@
         <v>1.48</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
@@ -564,13 +564,13 @@
         <v>1.49</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="F6" t="n">
         <v>1.2</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.86</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
         <v>1.16</v>

</xml_diff>

<commit_message>
spring 24 week 12 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,10 +466,10 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
       <c r="E2" t="n">
         <v>1.16</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.52</v>
+        <v>1.53</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="C4" t="n">
         <v>1.43</v>
@@ -518,13 +518,13 @@
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
         <v>1.11</v>
       </c>
       <c r="G4" t="n">
-        <v>0.97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -538,10 +538,10 @@
         <v>1.32</v>
       </c>
       <c r="D5" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F5" t="n">
         <v>1.05</v>
@@ -570,7 +570,7 @@
         <v>1.2</v>
       </c>
       <c r="G6" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>2.18</v>
       </c>
       <c r="D7" t="n">
-        <v>1.76</v>
+        <v>1.73</v>
       </c>
       <c r="E7" t="n">
         <v>1.86</v>

</xml_diff>

<commit_message>
spring 24 week 13 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.31</v>
       </c>
       <c r="D2" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="E2" t="n">
         <v>1.16</v>
@@ -495,7 +495,7 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.32</v>
+        <v>1.34</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.45</v>
+        <v>1.48</v>
       </c>
       <c r="C4" t="n">
         <v>1.43</v>
@@ -535,13 +535,13 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="F5" t="n">
         <v>1.05</v>
@@ -587,7 +587,7 @@
         <v>1.73</v>
       </c>
       <c r="E7" t="n">
-        <v>1.86</v>
+        <v>1.87</v>
       </c>
       <c r="F7" t="n">
         <v>1.47</v>

</xml_diff>

<commit_message>
spring 24 week 14 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.31</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="E2" t="n">
         <v>1.16</v>
@@ -492,10 +492,10 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="E3" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.48</v>
+        <v>1.5</v>
       </c>
       <c r="C4" t="n">
         <v>1.43</v>
@@ -521,7 +521,7 @@
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.11</v>
+        <v>1.1</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -535,7 +535,7 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.31</v>
+        <v>1.34</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -544,7 +544,7 @@
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="G5" t="n">
         <v>0.78</v>
@@ -570,7 +570,7 @@
         <v>1.2</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.87</v>
       </c>
       <c r="F7" t="n">
-        <v>1.47</v>
+        <v>1.49</v>
       </c>
       <c r="G7" t="n">
         <v>1.16</v>

</xml_diff>

<commit_message>
spring 24 week 15 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="D2" t="n">
         <v>1.24</v>
@@ -486,19 +486,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.53</v>
+        <v>1.54</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F3" t="n">
-        <v>1.2</v>
+        <v>1.21</v>
       </c>
       <c r="G3" t="n">
         <v>0.64</v>
@@ -512,13 +512,13 @@
         <v>1.5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
@@ -535,10 +535,10 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -558,7 +558,7 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="D6" t="n">
         <v>1.49</v>
@@ -593,7 +593,7 @@
         <v>1.49</v>
       </c>
       <c r="G7" t="n">
-        <v>1.16</v>
+        <v>1.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spring 24 reg season complete
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -498,7 +498,7 @@
         <v>1.32</v>
       </c>
       <c r="F3" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="G3" t="n">
         <v>0.64</v>
@@ -524,7 +524,7 @@
         <v>1.1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="5">
@@ -538,7 +538,7 @@
         <v>1.35</v>
       </c>
       <c r="D5" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -570,7 +570,7 @@
         <v>1.2</v>
       </c>
       <c r="G6" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="7">
@@ -584,13 +584,13 @@
         <v>2.18</v>
       </c>
       <c r="D7" t="n">
-        <v>1.73</v>
+        <v>1.68</v>
       </c>
       <c r="E7" t="n">
         <v>1.87</v>
       </c>
       <c r="F7" t="n">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
summer 24 week 1 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.3</v>
+        <v>1.31</v>
       </c>
       <c r="D2" t="n">
         <v>1.24</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.54</v>
+        <v>1.53</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,10 +495,10 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="G3" t="n">
         <v>0.64</v>
@@ -521,7 +521,7 @@
         <v>1.23</v>
       </c>
       <c r="F4" t="n">
-        <v>1.1</v>
+        <v>1.12</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -535,7 +535,7 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -558,10 +558,10 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.45</v>
+        <v>1.48</v>
       </c>
       <c r="D6" t="n">
-        <v>1.49</v>
+        <v>1.48</v>
       </c>
       <c r="E6" t="n">
         <v>1.31</v>
@@ -570,7 +570,7 @@
         <v>1.2</v>
       </c>
       <c r="G6" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.87</v>
       </c>
       <c r="F7" t="n">
-        <v>1.5</v>
+        <v>1.48</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
summer 24 week 3 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,10 +492,10 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="E3" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -535,7 +535,7 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -567,7 +567,7 @@
         <v>1.31</v>
       </c>
       <c r="F6" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="G6" t="n">
         <v>0.98</v>

</xml_diff>

<commit_message>
summer 24 week 5 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="D2" t="n">
         <v>1.24</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.53</v>
+        <v>1.54</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,7 +495,7 @@
         <v>1.41</v>
       </c>
       <c r="E3" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -512,16 +512,16 @@
         <v>1.5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -535,7 +535,7 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -544,7 +544,7 @@
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="G5" t="n">
         <v>0.78</v>
@@ -561,10 +561,10 @@
         <v>1.48</v>
       </c>
       <c r="D6" t="n">
-        <v>1.48</v>
+        <v>1.5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.31</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
summer 24 week 5 updates
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,10 +466,10 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="D2" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="E2" t="n">
         <v>1.16</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.54</v>
+        <v>1.55</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,7 +495,7 @@
         <v>1.41</v>
       </c>
       <c r="E3" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -509,10 +509,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.5</v>
+        <v>1.51</v>
       </c>
       <c r="C4" t="n">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
@@ -535,10 +535,10 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="D5" t="n">
         <v>1.33</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -558,7 +558,7 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="D6" t="n">
         <v>1.5</v>

</xml_diff>

<commit_message>
summer 24 week 7 updates
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="D2" t="n">
         <v>1.23</v>
       </c>
       <c r="E2" t="n">
-        <v>1.16</v>
+        <v>1.19</v>
       </c>
       <c r="F2" t="n">
         <v>0.6899999999999999</v>
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
         <v>1.32</v>
@@ -521,7 +521,7 @@
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.11</v>
+        <v>1.12</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -532,10 +532,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.58</v>
+        <v>1.53</v>
       </c>
       <c r="C5" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="D5" t="n">
         <v>1.33</v>
@@ -561,16 +561,16 @@
         <v>1.49</v>
       </c>
       <c r="D6" t="n">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.87</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
summer 24 week 8
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -472,7 +472,7 @@
         <v>1.23</v>
       </c>
       <c r="E2" t="n">
-        <v>1.19</v>
+        <v>1.15</v>
       </c>
       <c r="F2" t="n">
         <v>0.6899999999999999</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.55</v>
+        <v>1.54</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,13 +495,13 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="4">
@@ -512,16 +512,16 @@
         <v>1.51</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="F4" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -532,10 +532,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.53</v>
+        <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="D5" t="n">
         <v>1.33</v>
@@ -544,10 +544,10 @@
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="6">
@@ -561,10 +561,10 @@
         <v>1.49</v>
       </c>
       <c r="D6" t="n">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>
@@ -581,13 +581,13 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.18</v>
+        <v>2.17</v>
       </c>
       <c r="D7" t="n">
         <v>1.68</v>
       </c>
       <c r="E7" t="n">
-        <v>1.87</v>
+        <v>1.88</v>
       </c>
       <c r="F7" t="n">
         <v>1.49</v>

</xml_diff>

<commit_message>
summer 24 week 9 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="D2" t="n">
         <v>1.23</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.54</v>
+        <v>1.55</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,7 +495,7 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -518,7 +518,7 @@
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
         <v>1.11</v>
@@ -535,16 +535,16 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="D5" t="n">
         <v>1.34</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.33</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="G5" t="n">
         <v>0.77</v>
@@ -587,7 +587,7 @@
         <v>1.68</v>
       </c>
       <c r="E7" t="n">
-        <v>1.88</v>
+        <v>1.89</v>
       </c>
       <c r="F7" t="n">
         <v>1.49</v>

</xml_diff>

<commit_message>
summer 24 week 10 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="D2" t="n">
         <v>1.23</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.55</v>
+        <v>1.56</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -498,7 +498,7 @@
         <v>1.32</v>
       </c>
       <c r="F3" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="G3" t="n">
         <v>0.65</v>
@@ -512,7 +512,7 @@
         <v>1.51</v>
       </c>
       <c r="C4" t="n">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
       <c r="D4" t="n">
         <v>1.32</v>
@@ -521,7 +521,7 @@
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.11</v>
+        <v>1.1</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -558,10 +558,10 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.49</v>
+        <v>1.51</v>
       </c>
       <c r="D6" t="n">
-        <v>1.5</v>
+        <v>1.51</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>
@@ -590,7 +590,7 @@
         <v>1.89</v>
       </c>
       <c r="F7" t="n">
-        <v>1.49</v>
+        <v>1.48</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
summer 24 week 11 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.28</v>
       </c>
       <c r="D2" t="n">
-        <v>1.23</v>
+        <v>1.26</v>
       </c>
       <c r="E2" t="n">
         <v>1.15</v>
@@ -495,10 +495,10 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="F3" t="n">
-        <v>1.19</v>
+        <v>1.16</v>
       </c>
       <c r="G3" t="n">
         <v>0.65</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.51</v>
+        <v>1.49</v>
       </c>
       <c r="C4" t="n">
         <v>1.44</v>
@@ -518,7 +518,7 @@
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
@@ -535,10 +535,10 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -558,7 +558,7 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.51</v>
+        <v>1.55</v>
       </c>
       <c r="D6" t="n">
         <v>1.51</v>
@@ -570,7 +570,7 @@
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
summer 24 week 12 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
       <c r="D2" t="n">
         <v>1.26</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.56</v>
+        <v>1.55</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,7 +495,7 @@
         <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.31</v>
+        <v>1.29</v>
       </c>
       <c r="F3" t="n">
         <v>1.16</v>
@@ -535,16 +535,16 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.39</v>
       </c>
       <c r="D5" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="G5" t="n">
         <v>0.77</v>

</xml_diff>

<commit_message>
summer 24 week 13 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.29</v>
       </c>
       <c r="D2" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="E2" t="n">
         <v>1.15</v>
@@ -509,16 +509,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.49</v>
+        <v>1.46</v>
       </c>
       <c r="C4" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="D4" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
@@ -570,7 +570,7 @@
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="7">
@@ -590,7 +590,7 @@
         <v>1.89</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
summer 24 week 14 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -521,10 +521,10 @@
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.1</v>
+        <v>1.09</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -535,7 +535,7 @@
         <v>1.58</v>
       </c>
       <c r="C5" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
         <v>1.34</v>
@@ -561,7 +561,7 @@
         <v>1.55</v>
       </c>
       <c r="D6" t="n">
-        <v>1.51</v>
+        <v>1.53</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>
@@ -570,7 +570,7 @@
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>2.17</v>
       </c>
       <c r="D7" t="n">
-        <v>1.68</v>
+        <v>1.72</v>
       </c>
       <c r="E7" t="n">
         <v>1.89</v>

</xml_diff>

<commit_message>
summer 24 week 15 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -547,7 +547,7 @@
         <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.77</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="6">
@@ -564,7 +564,7 @@
         <v>1.53</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>
@@ -587,10 +587,10 @@
         <v>1.72</v>
       </c>
       <c r="E7" t="n">
-        <v>1.89</v>
+        <v>1.86</v>
       </c>
       <c r="F7" t="n">
-        <v>1.47</v>
+        <v>1.48</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
fall 24 week 2 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="D2" t="n">
         <v>1.27</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.55</v>
+        <v>1.56</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -495,13 +495,13 @@
         <v>1.39</v>
       </c>
       <c r="E3" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="F3" t="n">
-        <v>1.16</v>
+        <v>1.2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.09</v>
+        <v>1.1</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.58</v>
+        <v>1.59</v>
       </c>
       <c r="C5" t="n">
         <v>1.38</v>
@@ -547,7 +547,7 @@
         <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.79</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="6">
@@ -558,10 +558,10 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.55</v>
+        <v>1.52</v>
       </c>
       <c r="D6" t="n">
-        <v>1.53</v>
+        <v>1.51</v>
       </c>
       <c r="E6" t="n">
         <v>1.32</v>
@@ -590,7 +590,7 @@
         <v>1.86</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
fall 24 week 3 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -469,7 +469,7 @@
         <v>1.28</v>
       </c>
       <c r="D2" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="E2" t="n">
         <v>1.15</v>
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
         <v>1.3</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.46</v>
+        <v>1.49</v>
       </c>
       <c r="C4" t="n">
         <v>1.45</v>
@@ -518,7 +518,7 @@
         <v>1.33</v>
       </c>
       <c r="E4" t="n">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
@@ -535,10 +535,10 @@
         <v>1.59</v>
       </c>
       <c r="C5" t="n">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -564,7 +564,7 @@
         <v>1.51</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 24 week 4 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,16 +492,16 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="E3" t="n">
         <v>1.3</v>
       </c>
       <c r="F3" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.67</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="4">
@@ -515,7 +515,7 @@
         <v>1.45</v>
       </c>
       <c r="D4" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="E4" t="n">
         <v>1.21</v>
@@ -535,7 +535,7 @@
         <v>1.59</v>
       </c>
       <c r="C5" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
         <v>1.35</v>
@@ -547,7 +547,7 @@
         <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="6">
@@ -581,13 +581,13 @@
         <v>2.6</v>
       </c>
       <c r="C7" t="n">
-        <v>2.17</v>
+        <v>2.2</v>
       </c>
       <c r="D7" t="n">
         <v>1.72</v>
       </c>
       <c r="E7" t="n">
-        <v>1.86</v>
+        <v>1.87</v>
       </c>
       <c r="F7" t="n">
         <v>1.47</v>

</xml_diff>

<commit_message>
fall 24 week 5 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,13 +492,13 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="F3" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="G3" t="n">
         <v>0.64</v>
@@ -518,7 +518,7 @@
         <v>1.32</v>
       </c>
       <c r="E4" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
@@ -535,7 +535,7 @@
         <v>1.59</v>
       </c>
       <c r="C5" t="n">
-        <v>1.38</v>
+        <v>1.39</v>
       </c>
       <c r="D5" t="n">
         <v>1.35</v>
@@ -547,7 +547,7 @@
         <v>1.06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6">
@@ -558,13 +558,13 @@
         <v>2.12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="D6" t="n">
         <v>1.51</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>

</xml_diff>

<commit_message>
fall 24 week 6 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -492,7 +492,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="E3" t="n">
         <v>1.29</v>
@@ -515,7 +515,7 @@
         <v>1.45</v>
       </c>
       <c r="D4" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="E4" t="n">
         <v>1.22</v>
@@ -524,7 +524,7 @@
         <v>1.1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="5">
@@ -584,7 +584,7 @@
         <v>2.2</v>
       </c>
       <c r="D7" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="E7" t="n">
         <v>1.87</v>

</xml_diff>

<commit_message>
fall 24 week 8 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.28</v>
+        <v>1.27</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -512,7 +512,7 @@
         <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="D4" t="n">
         <v>1.33</v>
@@ -521,7 +521,7 @@
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -561,10 +561,10 @@
         <v>1.49</v>
       </c>
       <c r="D6" t="n">
-        <v>1.51</v>
+        <v>1.52</v>
       </c>
       <c r="E6" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>
@@ -593,7 +593,7 @@
         <v>1.47</v>
       </c>
       <c r="G7" t="n">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 24 week 10 inputs and lineup message improvements
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
@@ -475,7 +475,7 @@
         <v>1.15</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.83</v>
       </c>
       <c r="G2" t="n">
         <v>0.4</v>
@@ -486,13 +486,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.57</v>
+        <v>1.59</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="E3" t="n">
         <v>1.29</v>
@@ -512,16 +512,16 @@
         <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="D4" t="n">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="E4" t="n">
         <v>1.22</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08</v>
+        <v>1.09</v>
       </c>
       <c r="G4" t="n">
         <v>1.03</v>
@@ -538,7 +538,7 @@
         <v>1.39</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -555,13 +555,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>2.12</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>1.49</v>
       </c>
       <c r="D6" t="n">
-        <v>1.52</v>
+        <v>1.5</v>
       </c>
       <c r="E6" t="n">
         <v>1.33</v>
@@ -570,7 +570,7 @@
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="7">
@@ -590,10 +590,10 @@
         <v>1.87</v>
       </c>
       <c r="F7" t="n">
-        <v>1.47</v>
+        <v>1.48</v>
       </c>
       <c r="G7" t="n">
-        <v>1.14</v>
+        <v>1.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 24 week 13 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,13 +466,13 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
       </c>
       <c r="E2" t="n">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
       <c r="F2" t="n">
         <v>0.83</v>
@@ -486,13 +486,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.59</v>
+        <v>1.57</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="E3" t="n">
         <v>1.29</v>
@@ -515,7 +515,7 @@
         <v>1.47</v>
       </c>
       <c r="D4" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="E4" t="n">
         <v>1.22</v>
@@ -524,7 +524,7 @@
         <v>1.09</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="C5" t="n">
         <v>1.39</v>
@@ -564,7 +564,7 @@
         <v>1.5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="F6" t="n">
         <v>1.19</v>
@@ -584,7 +584,7 @@
         <v>2.2</v>
       </c>
       <c r="D7" t="n">
-        <v>1.67</v>
+        <v>1.71</v>
       </c>
       <c r="E7" t="n">
         <v>1.87</v>

</xml_diff>

<commit_message>
fall 24 week 15 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
@@ -486,16 +486,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.57</v>
+        <v>1.59</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="E3" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="F3" t="n">
         <v>1.2</v>
@@ -535,19 +535,19 @@
         <v>1.6</v>
       </c>
       <c r="C5" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="D5" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
       </c>
       <c r="F5" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="G5" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6">
@@ -570,7 +570,7 @@
         <v>1.19</v>
       </c>
       <c r="G6" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>1.71</v>
       </c>
       <c r="E7" t="n">
-        <v>1.87</v>
+        <v>1.88</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>1.5</v>
       </c>
       <c r="G7" t="n">
         <v>1.15</v>

</xml_diff>

<commit_message>
fall 24 final inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchupAverages.xlsx
+++ b/data/SLMatchupAverages.xlsx
@@ -466,7 +466,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="D2" t="n">
         <v>1.25</v>
@@ -475,7 +475,7 @@
         <v>1.14</v>
       </c>
       <c r="F2" t="n">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="G2" t="n">
         <v>0.4</v>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.59</v>
+        <v>1.58</v>
       </c>
       <c r="C3" t="n">
         <v>1.5</v>
@@ -498,7 +498,7 @@
         <v>1.3</v>
       </c>
       <c r="F3" t="n">
-        <v>1.2</v>
+        <v>1.23</v>
       </c>
       <c r="G3" t="n">
         <v>0.64</v>
@@ -512,7 +512,7 @@
         <v>1.49</v>
       </c>
       <c r="C4" t="n">
-        <v>1.47</v>
+        <v>1.46</v>
       </c>
       <c r="D4" t="n">
         <v>1.33</v>
@@ -535,10 +535,10 @@
         <v>1.6</v>
       </c>
       <c r="C5" t="n">
-        <v>1.38</v>
+        <v>1.39</v>
       </c>
       <c r="D5" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="n">
         <v>1.21</v>
@@ -547,7 +547,7 @@
         <v>1.05</v>
       </c>
       <c r="G5" t="n">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="6">
@@ -555,10 +555,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="C6" t="n">
-        <v>1.49</v>
+        <v>1.47</v>
       </c>
       <c r="D6" t="n">
         <v>1.5</v>
@@ -593,7 +593,7 @@
         <v>1.5</v>
       </c>
       <c r="G7" t="n">
-        <v>1.15</v>
+        <v>1.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>